<commit_message>
add: add TD3 code and cls reg result
</commit_message>
<xml_diff>
--- a/results/Cls/cls_label_ml.xlsx
+++ b/results/Cls/cls_label_ml.xlsx
@@ -114,19 +114,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -177,21 +171,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -508,20 +499,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="22.5">
@@ -614,87 +605,87 @@
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.8022429821039202</v>
       </c>
-      <c r="C3" s="5">
-        <v>0.9692499335017392</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.9814031048334494</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.9805747143963227</v>
-      </c>
-      <c r="F3" s="5">
+      <c r="C3" s="4">
+        <v>0.969249933501739</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.981403104833449</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.980574714396323</v>
+      </c>
+      <c r="F3" s="4">
         <v>0.954888342219534</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0.9643701471094012</v>
       </c>
-      <c r="H3" s="5">
-        <v>0.9830598857077024</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="H3" s="4">
+        <v>0.983059885707702</v>
+      </c>
+      <c r="I3" s="4">
         <v>0.9627131968128273</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>0.5887503579046525</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>0.7124800716995261</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>0.8227722235493637</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>0.5881078237533482</v>
       </c>
-      <c r="N3" s="5">
-        <v>0.9825996499734855</v>
+      <c r="N3" s="4">
+        <v>0.982599649973486</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21.75">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.7929602544666895</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.9705048401373672</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.988072880583665</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.9844057647474452</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.9591503702344577</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>0.9497517682162793</v>
       </c>
-      <c r="H4" s="5">
-        <v>0.9873761453087833</v>
-      </c>
-      <c r="I4" s="5">
+      <c r="H4" s="4">
+        <v>0.987376145308783</v>
+      </c>
+      <c r="I4" s="4">
         <v>0.9675545659081026</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>0.8904024790595535</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>0.7213059363984466</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>0.8158114222257244</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>0.9484196173405783</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>0.9855563812590475</v>
       </c>
     </row>
@@ -702,43 +693,43 @@
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>0.8186313726088157</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.9679610531969145</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.9745898709171339</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.9766158230282207</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.950284883632279</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.9806656941825459</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>0.9786407586053834</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>0.9576500107583172</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>0.2023583587043259</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>0.6921327051153681</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>0.8339103857576822</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>0.1863428667273199</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>0.9795610606514966</v>
       </c>
     </row>
@@ -746,44 +737,44 @@
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>0.8054455549992324</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.9692094320368996</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.9812652951250775</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.9804897029675912</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.9546735604649458</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0.9649529201003093</v>
       </c>
-      <c r="H6" s="5">
-        <v>0.9829827108806007</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="H6" s="4">
+        <v>0.982982710880601</v>
+      </c>
+      <c r="I6" s="4">
         <v>0.9625299161595429</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>0.3296717039022842</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>0.7061749539545771</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>0.8246057795887338</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>0.311092360359856</v>
       </c>
-      <c r="N6" s="5">
-        <v>0.9825428387931451</v>
+      <c r="N6" s="4">
+        <v>0.982542838793145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: add ppo and td3 train code
</commit_message>
<xml_diff>
--- a/results/Cls/cls_label_ml.xlsx
+++ b/results/Cls/cls_label_ml.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>LogisticRegression</t>
   </si>
@@ -49,6 +49,9 @@
     <t>BernoulliNB</t>
   </si>
   <si>
+    <t>LinearDiscriminantAnalysis</t>
+  </si>
+  <si>
     <t>QuadraticDiscriminantAnalysis</t>
   </si>
   <si>
@@ -58,43 +61,46 @@
     <t>best_params</t>
   </si>
   <si>
-    <t>{'C': 0.001, 'class_weight': 'balanced', 'max_iter': 5000, 'penalty': 'none', 'solver': 'lbfgs'}</t>
+    <t>{'C': 100, 'class_weight': 'balanced', 'max_iter': 5000, 'penalty': 'l1', 'solver': 'liblinear'}</t>
   </si>
   <si>
     <t>{'C': 100, 'class_weight': 'balanced', 'degree': 5, 'gamma': 'scale', 'kernel': 'poly'}</t>
   </si>
   <si>
-    <t>{'class_weight': 'balanced', 'max_depth': 30, 'max_features': 'sqrt', 'n_estimators': 500}</t>
-  </si>
-  <si>
-    <t>{'learning_rate': 0.5, 'max_depth': 15, 'n_estimators': 500}</t>
-  </si>
-  <si>
-    <t>{'learning_rate': 1, 'n_estimators': 500}</t>
-  </si>
-  <si>
-    <t>{'algorithm': 'auto', 'n_neighbors': 10, 'weights': 'distance'}</t>
-  </si>
-  <si>
-    <t>{'colsample_bytree': 0.75, 'learning_rate': 0.05, 'max_depth': 20, 'n_estimators': 500, 'subsample': 0.75}</t>
-  </si>
-  <si>
-    <t>{'class_weight': 'balanced', 'max_depth': None, 'min_samples_leaf': 2, 'min_samples_split': 20}</t>
-  </si>
-  <si>
-    <t>{'var_smoothing': 1e-10}</t>
+    <t>{'class_weight': 'balanced', 'max_depth': 30, 'max_features': 'log2', 'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>{'learning_rate': 0.1, 'max_depth': 15, 'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>{'learning_rate': 1, 'n_estimators': 200}</t>
+  </si>
+  <si>
+    <t>{'algorithm': 'kd_tree', 'n_neighbors': 20, 'weights': 'distance'}</t>
+  </si>
+  <si>
+    <t>{'colsample_bytree': 1, 'learning_rate': 0.2, 'max_depth': 15, 'n_estimators': 100, 'subsample': 0.75}</t>
+  </si>
+  <si>
+    <t>{'class_weight': 'balanced', 'max_depth': None, 'min_samples_leaf': 10, 'min_samples_split': 2}</t>
+  </si>
+  <si>
+    <t>{'var_smoothing': 1e-09}</t>
   </si>
   <si>
     <t>{'alpha': 0.001}</t>
   </si>
   <si>
-    <t>{'alpha': 1}</t>
-  </si>
-  <si>
-    <t>{'reg_param': 0}</t>
-  </si>
-  <si>
-    <t>{'depth': 12, 'iterations': 1000, 'learning_rate': 0.2}</t>
+    <t>{'alpha': 10}</t>
+  </si>
+  <si>
+    <t>{'shrinkage': None, 'solver': 'svd'}</t>
+  </si>
+  <si>
+    <t>{'reg_param': 0.001}</t>
+  </si>
+  <si>
+    <t>{'depth': 12, 'iterations': 500, 'learning_rate': 0.05}</t>
   </si>
   <si>
     <t>auc</t>
@@ -114,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,7 +130,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -138,13 +150,6 @@
     </fill>
   </fills>
   <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
     <border>
       <left/>
       <right/>
@@ -167,22 +172,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -493,29 +508,30 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -556,225 +572,243 @@
       <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.8022429821039202</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.969249933501739</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.981403104833449</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.980574714396323</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.954888342219534</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.9643701471094012</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.983059885707702</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0.9627131968128273</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0.5887503579046525</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0.7124800716995261</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0.8227722235493637</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0.5881078237533482</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0.982599649973486</v>
+        <v>29</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.7895692660794115</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.9447236139259851</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.951285338492861</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.945789890243625</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.9161517035445215</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.9334629879390196</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.953228099025248</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.9159221515897429</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.5910033437574579</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0.7041915230739697</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.7920668252054273</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0.7754366643534378</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0.7899757642523814</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0.955344336054088</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.7929602544666895</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.9705048401373672</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.988072880583665</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.9844057647474452</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.9591503702344577</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.9497517682162793</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.987376145308783</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0.9675545659081026</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0.8904024790595535</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0.7213059363984466</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0.8158114222257244</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0.9484196173405783</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0.9855563812590475</v>
+        <v>30</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.4929377287384916</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.8843373527858998</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.9583357669752743</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.9351493853552645</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.8326521251637532</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.7868308604310836</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.9471694593685435</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.8481171014811035</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.6569308500099069</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.3984345644089635</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.5450368526624689</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.4659598248453413</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0.4615638553986353</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.9496624863201628</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.8186313726088157</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.9679610531969145</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.9745898709171339</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.9766158230282207</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.950284883632279</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.9806656941825459</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0.9786407586053834</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0.9576500107583172</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0.2023583587043259</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0.6921327051153681</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0.8339103857576822</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0.1863428667273199</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0.9795610606514966</v>
+        <v>31</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.7938338854128328</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.9214844804318488</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.913065881486934</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.9081511470985155</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.8787044534412957</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.9333971291866028</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.920080971659919</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.873087964666912</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.2110980247822353</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0.6773990921359342</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.7489314194577353</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0.7882173966384493</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0.8366310882100356</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.9235774751564223</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.8054455549992324</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.9692094320368996</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.9812652951250775</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.9804897029675912</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.9546735604649458</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.9649529201003093</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.982982710880601</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0.9625299161595429</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0.3296717039022842</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0.7061749539545771</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0.8246057795887338</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0.311092360359856</v>
-      </c>
-      <c r="N6" s="4">
-        <v>0.982542838793145</v>
+        <v>32</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.608085592813657</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.9018777352368484</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.9348811096278176</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.9212492399836778</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.8549746141047103</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.8538004635340825</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.9330847165080967</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.8602059814917343</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.3191187349385533</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0.5014362719568245</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.6303613613361694</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.5854660585677223</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0.5948105356721952</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0.9363110323796331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: add new search results
</commit_message>
<xml_diff>
--- a/results/Cls/cls_label_ml.xlsx
+++ b/results/Cls/cls_label_ml.xlsx
@@ -120,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,13 +130,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -150,6 +144,13 @@
     </fill>
   </fills>
   <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -172,32 +173,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -514,24 +505,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="22.5">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -576,7 +567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21.75">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -623,192 +614,192 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21.75">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.7895692660794115</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.9447236139259851</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.951285338492861</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.945789890243625</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.9161517035445215</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0.9334629879390196</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>0.953228099025248</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>0.9159221515897429</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>0.5910033437574579</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>0.7041915230739697</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>0.7920668252054273</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>0.7754366643534378</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="4">
         <v>0.7899757642523814</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="4">
         <v>0.955344336054088</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21.75">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.4929377287384916</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.8843373527858998</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.9583357669752743</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.9351493853552645</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.8326521251637532</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>0.7868308604310836</v>
       </c>
-      <c r="H4" s="5">
-        <v>0.9471694593685435</v>
-      </c>
-      <c r="I4" s="5">
+      <c r="H4" s="4">
+        <v>0.947169459368544</v>
+      </c>
+      <c r="I4" s="4">
         <v>0.8481171014811035</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>0.6569308500099069</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>0.3984345644089635</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>0.5450368526624689</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>0.4659598248453413</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>0.4615638553986353</v>
       </c>
-      <c r="O4" s="5">
-        <v>0.9496624863201628</v>
+      <c r="O4" s="4">
+        <v>0.949662486320163</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21.75">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>0.7938338854128328</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.9214844804318488</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.913065881486934</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.9081511470985155</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.8787044534412957</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.9333971291866028</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>0.920080971659919</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>0.873087964666912</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>0.2110980247822353</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>0.6773990921359342</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>0.7489314194577353</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>0.7882173966384493</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>0.8366310882100356</v>
       </c>
-      <c r="O5" s="5">
-        <v>0.9235774751564223</v>
+      <c r="O5" s="4">
+        <v>0.923577475156422</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="22.5">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>0.608085592813657</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.9018777352368484</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.9348811096278176</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.9212492399836778</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.8549746141047103</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0.8538004635340825</v>
       </c>
-      <c r="H6" s="5">
-        <v>0.9330847165080967</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="H6" s="4">
+        <v>0.933084716508097</v>
+      </c>
+      <c r="I6" s="4">
         <v>0.8602059814917343</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>0.3191187349385533</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>0.5014362719568245</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>0.6303613613361694</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>0.5854660585677223</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <v>0.5948105356721952</v>
       </c>
-      <c r="O6" s="5">
-        <v>0.9363110323796331</v>
+      <c r="O6" s="4">
+        <v>0.936311032379633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: add new design results
</commit_message>
<xml_diff>
--- a/results/Cls/cls_label_ml.xlsx
+++ b/results/Cls/cls_label_ml.xlsx
@@ -61,31 +61,31 @@
     <t>best_params</t>
   </si>
   <si>
-    <t>{'C': 100, 'class_weight': 'balanced', 'max_iter': 5000, 'penalty': 'l1', 'solver': 'liblinear'}</t>
+    <t>{'C': 0.001, 'class_weight': 'balanced', 'max_iter': 1000, 'penalty': 'none', 'solver': 'lbfgs'}</t>
   </si>
   <si>
     <t>{'C': 100, 'class_weight': 'balanced', 'degree': 5, 'gamma': 'scale', 'kernel': 'poly'}</t>
   </si>
   <si>
-    <t>{'class_weight': 'balanced', 'max_depth': 30, 'max_features': 'log2', 'n_estimators': 200}</t>
+    <t>{'class_weight': 'balanced', 'max_depth': 30, 'max_features': 'sqrt', 'n_estimators': 500}</t>
   </si>
   <si>
     <t>{'learning_rate': 0.1, 'max_depth': 15, 'n_estimators': 200}</t>
   </si>
   <si>
-    <t>{'learning_rate': 1, 'n_estimators': 200}</t>
-  </si>
-  <si>
-    <t>{'algorithm': 'kd_tree', 'n_neighbors': 20, 'weights': 'distance'}</t>
-  </si>
-  <si>
-    <t>{'colsample_bytree': 1, 'learning_rate': 0.2, 'max_depth': 15, 'n_estimators': 100, 'subsample': 0.75}</t>
-  </si>
-  <si>
-    <t>{'class_weight': 'balanced', 'max_depth': None, 'min_samples_leaf': 10, 'min_samples_split': 2}</t>
-  </si>
-  <si>
-    <t>{'var_smoothing': 1e-09}</t>
+    <t>{'learning_rate': 0.5, 'n_estimators': 500}</t>
+  </si>
+  <si>
+    <t>{'algorithm': 'auto', 'n_neighbors': 20, 'weights': 'distance'}</t>
+  </si>
+  <si>
+    <t>{'colsample_bytree': 1, 'learning_rate': 0.1, 'max_depth': 20, 'n_estimators': 500, 'subsample': 1}</t>
+  </si>
+  <si>
+    <t>{'class_weight': 'balanced', 'max_depth': None, 'min_samples_leaf': 10, 'min_samples_split': 10}</t>
+  </si>
+  <si>
+    <t>{'var_smoothing': 1e-10}</t>
   </si>
   <si>
     <t>{'alpha': 0.001}</t>
@@ -97,10 +97,10 @@
     <t>{'shrinkage': None, 'solver': 'svd'}</t>
   </si>
   <si>
-    <t>{'reg_param': 0.001}</t>
-  </si>
-  <si>
-    <t>{'depth': 12, 'iterations': 500, 'learning_rate': 0.05}</t>
+    <t>{'reg_param': 0}</t>
+  </si>
+  <si>
+    <t>{'depth': 12, 'iterations': 200, 'learning_rate': 0.3}</t>
   </si>
   <si>
     <t>auc</t>
@@ -120,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,7 +130,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -144,13 +150,6 @@
     </fill>
   </fills>
   <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
     <border>
       <left/>
       <right/>
@@ -173,22 +172,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -505,24 +514,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -567,7 +576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -614,192 +623,192 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.7895692660794115</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.9447236139259851</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.951285338492861</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.945789890243625</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.9161517035445215</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.9334629879390196</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.953228099025248</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0.9159221515897429</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0.5910033437574579</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0.7041915230739697</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0.7920668252054273</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0.7754366643534378</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0.7899757642523814</v>
-      </c>
-      <c r="O3" s="4">
-        <v>0.955344336054088</v>
+      <c r="B3" s="5">
+        <v>0.7914458744474995</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.9504235055728387</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.9551778530015715</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.949493917991761</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.9209160017644841</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.9346438746952928</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.9544603172409628</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.9083405028241327</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.5877115778525376</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0.7066571001307416</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.7946013058723489</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0.7761606994404916</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0.582441004383633</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0.9558674225081324</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="4">
-        <v>0.4929377287384916</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.8843373527858998</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.9583357669752743</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.9351493853552645</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.8326521251637532</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.7868308604310836</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.947169459368544</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0.8481171014811035</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0.6569308500099069</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0.3984345644089635</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0.5450368526624689</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0.4659598248453413</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0.4615638553986353</v>
-      </c>
-      <c r="O4" s="4">
-        <v>0.949662486320163</v>
+      <c r="B4" s="5">
+        <v>0.496864690339972</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.889228586006403</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.9627451296403222</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.9359189168329489</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.8389735690292397</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.786386343258788</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.9470553201389548</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.8451065092640991</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.7024022318502933</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.4002581840138857</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.5467456878537378</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.4682937741067413</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0.8266731915427566</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.949876312866869</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="4">
-        <v>0.7938338854128328</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.9214844804318488</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.913065881486934</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.9081511470985155</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.8787044534412957</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.9333971291866028</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0.920080971659919</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0.873087964666912</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0.2110980247822353</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0.6773990921359342</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0.7489314194577353</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0.7882173966384493</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0.8366310882100356</v>
-      </c>
-      <c r="O5" s="4">
-        <v>0.923577475156422</v>
+      <c r="B5" s="5">
+        <v>0.7955581004361492</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.931597670622061</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.9197461075509856</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.9155600497063912</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.8869447625545186</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.9364952121049681</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.9225457469359908</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.8582953631734119</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.1975195536171146</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0.6825101727540752</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.7543651470480739</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0.788557783679735</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0.1744572500670062</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.9246241563314733</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="4">
-        <v>0.608085592813657</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.9018777352368484</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.9348811096278176</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.9212492399836778</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.8549746141047103</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.8538004635340825</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.933084716508097</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0.8602059814917343</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0.3191187349385533</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0.5014362719568245</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0.6303613613361694</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0.5854660585677223</v>
-      </c>
-      <c r="N6" s="4">
-        <v>0.5948105356721952</v>
-      </c>
-      <c r="O6" s="4">
-        <v>0.936311032379633</v>
+      <c r="B6" s="5">
+        <v>0.6115565128632438</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.9096988520356126</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.9407415910917232</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.9255762560598644</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.8620438453164787</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.854849899131097</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.9346178937691045</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.8511453806981898</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.307964765271255</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0.5042643868842799</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.6338902267639352</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.5875148290025721</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0.2863870178062579</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0.9370465369300087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: add new ML and cls results
</commit_message>
<xml_diff>
--- a/results/Cls/cls_label_ml.xlsx
+++ b/results/Cls/cls_label_ml.xlsx
@@ -634,7 +634,7 @@
         <v>0.9504235055728387</v>
       </c>
       <c r="D3" s="5">
-        <v>0.9551778530015715</v>
+        <v>0.955177853001572</v>
       </c>
       <c r="E3" s="5">
         <v>0.949493917991761</v>
@@ -646,7 +646,7 @@
         <v>0.9346438746952928</v>
       </c>
       <c r="H3" s="5">
-        <v>0.9544603172409628</v>
+        <v>0.954460317240963</v>
       </c>
       <c r="I3" s="5">
         <v>0.9083405028241327</v>
@@ -667,7 +667,7 @@
         <v>0.582441004383633</v>
       </c>
       <c r="O3" s="5">
-        <v>0.9558674225081324</v>
+        <v>0.955867422508132</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">

</xml_diff>